<commit_message>
- typo fix in property name (`superconducting critical temperature`)
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jul2025.xlsx
+++ b/MiscSmallUploads_Jul2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BCFEEF-CCAF-264A-8367-0EDDEDA6B84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9683698-4AA1-3945-9978-9C68EF862D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="7300" windowWidth="31960" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="6580" windowWidth="31960" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -411,9 +411,6 @@
     <t>annealed at 1073K for 96h (best of 3 annealing trials in the paper); equal BCC and FCC fractions</t>
   </si>
   <si>
-    <t>superconducting critical temperature</t>
-  </si>
-  <si>
     <t>K</t>
   </si>
   <si>
@@ -427,6 +424,9 @@
   </si>
   <si>
     <t>F3</t>
+  </si>
+  <si>
+    <t>superconducting transition temperature</t>
   </si>
 </sst>
 </file>
@@ -1663,57 +1663,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1773,6 +1722,57 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2937,7 +2937,7 @@
   <dimension ref="A1:T960"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -2994,19 +2994,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="129" t="s">
+      <c r="D2" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="130"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="134"/>
-      <c r="M2" s="134"/>
-      <c r="N2" s="137"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
+      <c r="N2" s="120"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -3022,17 +3022,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="131"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138"/>
-      <c r="I3" s="139"/>
-      <c r="J3" s="140"/>
-      <c r="K3" s="140"/>
-      <c r="L3" s="138"/>
-      <c r="M3" s="138"/>
-      <c r="N3" s="141"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="121"/>
+      <c r="M3" s="121"/>
+      <c r="N3" s="124"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -3073,43 +3073,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="142" t="s">
+      <c r="C5" s="125" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="144" t="s">
+      <c r="D5" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="144" t="s">
+      <c r="E5" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="144" t="s">
+      <c r="F5" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="144" t="s">
+      <c r="G5" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="145" t="s">
+      <c r="H5" s="128" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="144" t="s">
+      <c r="I5" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="144" t="s">
+      <c r="J5" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="144" t="s">
+      <c r="K5" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="144" t="s">
+      <c r="L5" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="144" t="s">
+      <c r="M5" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="144" t="s">
+      <c r="N5" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="112" t="s">
+      <c r="O5" s="132" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3125,19 +3125,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="143"/>
-      <c r="D6" s="143"/>
-      <c r="E6" s="143"/>
-      <c r="F6" s="143"/>
-      <c r="G6" s="143"/>
-      <c r="H6" s="146"/>
-      <c r="I6" s="147"/>
-      <c r="J6" s="148"/>
-      <c r="K6" s="148"/>
-      <c r="L6" s="143"/>
-      <c r="M6" s="143"/>
-      <c r="N6" s="143"/>
-      <c r="O6" s="113"/>
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="131"/>
+      <c r="K6" s="131"/>
+      <c r="L6" s="126"/>
+      <c r="M6" s="126"/>
+      <c r="N6" s="126"/>
+      <c r="O6" s="133"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3187,7 +3187,7 @@
       <c r="N7" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="114"/>
+      <c r="O7" s="134"/>
       <c r="P7" s="68" t="s">
         <v>62</v>
       </c>
@@ -3202,35 +3202,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" thickBot="1">
       <c r="A8" s="63"/>
-      <c r="B8" s="115" t="s">
+      <c r="B8" s="135" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="116"/>
-      <c r="D8" s="116"/>
-      <c r="E8" s="117"/>
-      <c r="F8" s="118" t="s">
+      <c r="C8" s="136"/>
+      <c r="D8" s="136"/>
+      <c r="E8" s="137"/>
+      <c r="F8" s="138" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="119"/>
-      <c r="H8" s="119"/>
-      <c r="I8" s="120"/>
-      <c r="J8" s="121"/>
-      <c r="K8" s="121"/>
-      <c r="L8" s="122"/>
-      <c r="M8" s="123" t="s">
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="140"/>
+      <c r="J8" s="141"/>
+      <c r="K8" s="141"/>
+      <c r="L8" s="142"/>
+      <c r="M8" s="143" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="124"/>
+      <c r="N8" s="144"/>
       <c r="O8" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="125" t="s">
+      <c r="P8" s="145" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="126"/>
-      <c r="R8" s="127"/>
-      <c r="S8" s="127"/>
-      <c r="T8" s="128"/>
+      <c r="Q8" s="146"/>
+      <c r="R8" s="147"/>
+      <c r="S8" s="147"/>
+      <c r="T8" s="148"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="64" t="s">
@@ -3723,7 +3723,7 @@
         <v>91</v>
       </c>
       <c r="F18" s="32" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="G18" s="73" t="s">
         <v>29</v>
@@ -3735,10 +3735,10 @@
       </c>
       <c r="K18" s="38"/>
       <c r="L18" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="M18" s="32" t="s">
         <v>94</v>
-      </c>
-      <c r="M18" s="32" t="s">
-        <v>95</v>
       </c>
       <c r="N18" s="76" t="s">
         <v>86</v>
@@ -3765,7 +3765,7 @@
         <v>92</v>
       </c>
       <c r="F19" s="32" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="G19" s="73" t="s">
         <v>29</v>
@@ -3777,10 +3777,10 @@
       </c>
       <c r="K19" s="38"/>
       <c r="L19" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="M19" s="32" t="s">
         <v>94</v>
-      </c>
-      <c r="M19" s="32" t="s">
-        <v>95</v>
       </c>
       <c r="N19" s="76" t="s">
         <v>86</v>
@@ -3807,7 +3807,7 @@
         <v>91</v>
       </c>
       <c r="F20" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G20" s="73" t="s">
         <v>29</v>
@@ -3821,10 +3821,10 @@
       </c>
       <c r="K20" s="38"/>
       <c r="L20" s="73" t="s">
+        <v>96</v>
+      </c>
+      <c r="M20" s="32" t="s">
         <v>97</v>
-      </c>
-      <c r="M20" s="32" t="s">
-        <v>98</v>
       </c>
       <c r="N20" s="76" t="s">
         <v>86</v>
@@ -3851,7 +3851,7 @@
         <v>92</v>
       </c>
       <c r="F21" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G21" s="73" t="s">
         <v>29</v>
@@ -3865,10 +3865,10 @@
       </c>
       <c r="K21" s="38"/>
       <c r="L21" s="73" t="s">
+        <v>96</v>
+      </c>
+      <c r="M21" s="32" t="s">
         <v>97</v>
-      </c>
-      <c r="M21" s="32" t="s">
-        <v>98</v>
       </c>
       <c r="N21" s="76" t="s">
         <v>86</v>
@@ -3895,7 +3895,7 @@
         <v>91</v>
       </c>
       <c r="F22" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G22" s="73" t="s">
         <v>29</v>
@@ -3909,10 +3909,10 @@
       </c>
       <c r="K22" s="35"/>
       <c r="L22" s="73" t="s">
+        <v>96</v>
+      </c>
+      <c r="M22" s="32" t="s">
         <v>97</v>
-      </c>
-      <c r="M22" s="32" t="s">
-        <v>98</v>
       </c>
       <c r="N22" s="76" t="s">
         <v>86</v>
@@ -3939,7 +3939,7 @@
         <v>92</v>
       </c>
       <c r="F23" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G23" s="73" t="s">
         <v>29</v>
@@ -3953,10 +3953,10 @@
       </c>
       <c r="K23" s="62"/>
       <c r="L23" s="73" t="s">
+        <v>96</v>
+      </c>
+      <c r="M23" s="32" t="s">
         <v>97</v>
-      </c>
-      <c r="M23" s="32" t="s">
-        <v>98</v>
       </c>
       <c r="N23" s="76" t="s">
         <v>86</v>
@@ -3983,7 +3983,7 @@
         <v>91</v>
       </c>
       <c r="F24" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G24" s="73" t="s">
         <v>29</v>
@@ -3997,10 +3997,10 @@
       </c>
       <c r="K24" s="62"/>
       <c r="L24" s="73" t="s">
+        <v>96</v>
+      </c>
+      <c r="M24" s="32" t="s">
         <v>97</v>
-      </c>
-      <c r="M24" s="32" t="s">
-        <v>98</v>
       </c>
       <c r="N24" s="76" t="s">
         <v>86</v>
@@ -4027,7 +4027,7 @@
         <v>92</v>
       </c>
       <c r="F25" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G25" s="73" t="s">
         <v>29</v>
@@ -4041,10 +4041,10 @@
       </c>
       <c r="K25" s="62"/>
       <c r="L25" s="73" t="s">
+        <v>96</v>
+      </c>
+      <c r="M25" s="32" t="s">
         <v>97</v>
-      </c>
-      <c r="M25" s="32" t="s">
-        <v>98</v>
       </c>
       <c r="N25" s="76" t="s">
         <v>86</v>
@@ -24486,6 +24486,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -24500,11 +24505,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>